<commit_message>
Anpassung Status Sprint1, Evaluation Sprint2
</commit_message>
<xml_diff>
--- a/doc/CS1/Task11/scrum_v02_sprint2.xlsx
+++ b/doc/CS1/Task11/scrum_v02_sprint2.xlsx
@@ -1102,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1191,7 +1191,7 @@
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -1223,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1319,7 +1319,39 @@
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2.1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2.4</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Presentation Task 11, Scrum Sprint 2
</commit_message>
<xml_diff>
--- a/doc/CS1/Task11/scrum_v02_sprint2.xlsx
+++ b/doc/CS1/Task11/scrum_v02_sprint2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -263,6 +263,39 @@
   </si>
   <si>
     <t>JPA - getting methods</t>
+  </si>
+  <si>
+    <t>Patient display</t>
+  </si>
+  <si>
+    <t>Medication display</t>
+  </si>
+  <si>
+    <t>Disgnosis display</t>
+  </si>
+  <si>
+    <t>laboraty display</t>
+  </si>
+  <si>
+    <t>schedule view</t>
+  </si>
+  <si>
+    <t>Database, JPA, Controller,UI</t>
+  </si>
+  <si>
+    <t>Shows in patient overview  information about patient</t>
+  </si>
+  <si>
+    <t>Shows in medication overview  information about medication</t>
+  </si>
+  <si>
+    <t>Shows in disgnosis overview  information about disgnosis</t>
+  </si>
+  <si>
+    <t>Shows in laboraty overview  information about laboraty</t>
+  </si>
+  <si>
+    <t>Shows in schedule overview  information about schedule</t>
   </si>
 </sst>
 </file>
@@ -693,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,7 +813,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1102,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,8 +1146,8 @@
     <col min="1" max="1" width="4.81640625" customWidth="1"/>
     <col min="2" max="2" width="6.1796875" customWidth="1"/>
     <col min="3" max="3" width="19.90625" customWidth="1"/>
-    <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="4" max="4" width="56.81640625" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" customWidth="1"/>
     <col min="6" max="6" width="14.54296875" customWidth="1"/>
     <col min="7" max="7" width="9.81640625" customWidth="1"/>
     <col min="8" max="8" width="8.36328125" customWidth="1"/>
@@ -1190,8 +1223,11 @@
       <c r="I2">
         <v>12</v>
       </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -1222,6 +1258,9 @@
       <c r="I3">
         <v>12</v>
       </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
       <c r="L3" t="s">
         <v>39</v>
       </c>
@@ -1254,6 +1293,9 @@
       <c r="I4">
         <v>6</v>
       </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
       <c r="L4" t="s">
         <v>40</v>
       </c>
@@ -1286,6 +1328,9 @@
       <c r="I5">
         <v>6</v>
       </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
       <c r="L5" t="s">
         <v>39</v>
       </c>
@@ -1318,8 +1363,11 @@
       <c r="I6">
         <v>6</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
       <c r="L6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1329,6 +1377,24 @@
       <c r="B7">
         <v>2</v>
       </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1337,6 +1403,24 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1345,6 +1429,24 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1352,6 +1454,53 @@
       </c>
       <c r="B10">
         <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2.5</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1524,7 @@
           <x14:formula1>
             <xm:f>excel_data!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H7</xm:sqref>
+          <xm:sqref>H2:H11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Presentation Scrum, Scrum avec sprint deux
</commit_message>
<xml_diff>
--- a/doc/CS1/Task11/scrum_v02_sprint2.xlsx
+++ b/doc/CS1/Task11/scrum_v02_sprint2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Remaining Effort</t>
   </si>
   <si>
-    <t>Remaining Ressources</t>
-  </si>
-  <si>
     <t>Fabian Kammermann</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>Shows in schedule overview  information about schedule</t>
+  </si>
+  <si>
+    <t>Remaining Resources</t>
   </si>
 </sst>
 </file>
@@ -383,9 +383,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,6 +401,1294 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>burndown-chart, blue</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Rmaining Effort</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-19A5-43A0-8F2A-3786DFAB24E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Remaining Ressources</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19A5-43A0-8F2A-3786DFAB24E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="549207312"/>
+        <c:axId val="549207640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="549207312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>calendar weeks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549207640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="549207640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Working hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549207312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>107389</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>102533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>555625</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97255450-11E7-4F0C-93C8-00E68EF0BB4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -746,58 +2034,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -812,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,10 +2147,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -871,7 +2159,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -879,10 +2167,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -891,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -899,16 +2187,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>38</v>
@@ -919,10 +2207,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -931,7 +2219,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -939,10 +2227,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -951,7 +2239,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -959,10 +2247,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -971,7 +2259,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -979,19 +2267,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -999,10 +2287,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1011,7 +2299,7 @@
         <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1019,10 +2307,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1031,7 +2319,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1039,10 +2327,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1051,7 +2339,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1059,10 +2347,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1071,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1079,10 +2367,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1091,12 +2379,12 @@
         <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1135,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1206,22 +2494,25 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2">
         <v>12</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
       </c>
       <c r="K2">
         <v>8</v>
@@ -1238,19 +2529,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -1258,11 +2549,14 @@
       <c r="I3">
         <v>12</v>
       </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
       <c r="K3">
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1273,19 +2567,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -1293,11 +2587,14 @@
       <c r="I4">
         <v>6</v>
       </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
       <c r="K4">
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1308,19 +2605,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
@@ -1328,11 +2625,14 @@
       <c r="I5">
         <v>6</v>
       </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
       <c r="K5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1343,19 +2643,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="s">
-        <v>75</v>
-      </c>
       <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
         <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -1363,11 +2663,14 @@
       <c r="I6">
         <v>6</v>
       </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1378,22 +2681,28 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -1404,22 +2713,28 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
         <v>5</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1430,22 +2745,28 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1456,22 +2777,28 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H10" t="s">
         <v>6</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1482,25 +2809,66 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" t="s">
-        <v>85</v>
-      </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2.6</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
         <v>5</v>
       </c>
-      <c r="I11">
-        <v>8</v>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <f>SUM(I7:I12)</f>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1512,19 +2880,19 @@
           <x14:formula1>
             <xm:f>ProjectTeam!$B$2:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F13 G2:G25</xm:sqref>
+          <xm:sqref>F8:F13 G8:G25 F2:G6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>excel_data!$B$3:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L9</xm:sqref>
+          <xm:sqref>L2:L12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>excel_data!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H11</xm:sqref>
+          <xm:sqref>H2:H12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1534,10 +2902,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,41 +2915,116 @@
     <col min="4" max="4" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="e">
-        <f>Wee</f>
-        <v>#NAME?</v>
+      <c r="B3" s="8">
+        <v>48</v>
       </c>
       <c r="C3">
+        <f>(5*42)</f>
         <v>210</v>
       </c>
       <c r="D3">
         <v>210</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="6"/>
+      <c r="F3">
+        <f>(7*6)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4" s="6">
+        <f>(C3-32)</f>
+        <v>178</v>
+      </c>
+      <c r="D4" s="6">
+        <f>(D3-42)</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:D9" si="0">(D4-42)</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1596,49 +3039,49 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="8" t="s">
-        <v>39</v>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="8" t="s">
-        <v>40</v>
+      <c r="B5" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B7" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="8" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>